<commit_message>
day-14 end of day update
</commit_message>
<xml_diff>
--- a/case study/Project groups.xlsx
+++ b/case study/Project groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\oracle\oracle-26thjuly2023\case study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0617E9B-4573-44A6-B3AA-EF7632796FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CFB911-453B-4DCF-B287-979191AB4AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA1A31B1-5E45-4749-8B39-4A461827EFAE}"/>
   </bookViews>
@@ -241,28 +241,28 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,7 +581,7 @@
   <dimension ref="A3:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,18 +592,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -620,7 +620,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="18">
         <v>1</v>
       </c>
       <c r="B6" s="1">
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -646,7 +646,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="19">
         <v>2</v>
       </c>
       <c r="B8" s="4">
@@ -655,24 +655,24 @@
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
+      <c r="A10" s="20">
         <v>3</v>
       </c>
       <c r="B10" s="6">
@@ -681,24 +681,24 @@
       <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="6">
         <v>2</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="21">
         <v>4</v>
       </c>
       <c r="B12" s="8">
@@ -707,24 +707,24 @@
       <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="8">
         <v>2</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="A14" s="22">
         <v>5</v>
       </c>
       <c r="B14" s="10">
@@ -733,42 +733,42 @@
       <c r="C14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="10">
         <v>2</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="10">
         <v>3</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="16" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A3:D4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{323A5CBA-7ACC-4A04-BC92-2BCD1E15BBE4}"/>

</xml_diff>